<commit_message>
Code changed on Feb 19
</commit_message>
<xml_diff>
--- a/testData/NinjaDataSheet.xlsx
+++ b/testData/NinjaDataSheet.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shada\OneDrive\Documents\CloudBerry\Batches\Jan 2025\Day 17\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7D525-2250-452F-8038-2D1237ED0BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1896" yWindow="1896" windowWidth="14400" windowHeight="8172"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -66,8 +60,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +83,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,15 +108,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -174,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -209,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -386,27 +393,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -414,15 +421,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -430,7 +437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -438,7 +445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -446,7 +453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -455,7 +462,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>